<commit_message>
initial app running. Added "pre/post election odds" column
</commit_message>
<xml_diff>
--- a/src/data/Election Odds Raw.xlsx
+++ b/src/data/Election Odds Raw.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Developer/2020-Election-Odds-Tracker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Developer/2020-Election-Odds-Tracker/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E4F789-4B40-D54D-BD16-A99F042664A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9BA914-1C24-FF43-884A-E6C2A322D1C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29400" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{E91F47DA-0CB0-014E-85A8-F4E87909AA65}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>date</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>source</t>
+  </si>
+  <si>
+    <t>pre_first_results</t>
   </si>
 </sst>
 </file>
@@ -397,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E09FD95-8348-4048-A5D2-30A6965E257B}">
-  <dimension ref="A1:D267"/>
+  <dimension ref="A1:E267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="A257" sqref="A257"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E218" sqref="E218:E267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,8 +421,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43929</v>
       </c>
@@ -432,8 +438,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43930</v>
       </c>
@@ -446,8 +455,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43931</v>
       </c>
@@ -460,8 +472,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43932</v>
       </c>
@@ -474,8 +489,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43933</v>
       </c>
@@ -488,8 +506,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43934</v>
       </c>
@@ -502,8 +523,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43935</v>
       </c>
@@ -516,8 +540,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43936</v>
       </c>
@@ -530,8 +557,11 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43937</v>
       </c>
@@ -544,8 +574,11 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43938</v>
       </c>
@@ -558,8 +591,11 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43939</v>
       </c>
@@ -572,8 +608,11 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43940</v>
       </c>
@@ -586,8 +625,11 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43941</v>
       </c>
@@ -600,8 +642,11 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43942</v>
       </c>
@@ -614,8 +659,11 @@
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43943</v>
       </c>
@@ -628,8 +676,11 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43944</v>
       </c>
@@ -642,8 +693,11 @@
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43945</v>
       </c>
@@ -656,8 +710,11 @@
       <c r="D18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43946</v>
       </c>
@@ -670,8 +727,11 @@
       <c r="D19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43947</v>
       </c>
@@ -684,8 +744,11 @@
       <c r="D20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43948</v>
       </c>
@@ -698,8 +761,11 @@
       <c r="D21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43949</v>
       </c>
@@ -712,8 +778,11 @@
       <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43950</v>
       </c>
@@ -726,8 +795,11 @@
       <c r="D23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43951</v>
       </c>
@@ -740,8 +812,11 @@
       <c r="D24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43952</v>
       </c>
@@ -754,8 +829,11 @@
       <c r="D25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43953</v>
       </c>
@@ -768,8 +846,11 @@
       <c r="D26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43954</v>
       </c>
@@ -782,8 +863,11 @@
       <c r="D27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43955</v>
       </c>
@@ -796,8 +880,11 @@
       <c r="D28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43956</v>
       </c>
@@ -810,8 +897,11 @@
       <c r="D29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43957</v>
       </c>
@@ -824,8 +914,11 @@
       <c r="D30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43958</v>
       </c>
@@ -838,8 +931,11 @@
       <c r="D31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43959</v>
       </c>
@@ -852,8 +948,11 @@
       <c r="D32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43960</v>
       </c>
@@ -866,8 +965,11 @@
       <c r="D33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43961</v>
       </c>
@@ -880,8 +982,11 @@
       <c r="D34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43962</v>
       </c>
@@ -894,8 +999,11 @@
       <c r="D35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43963</v>
       </c>
@@ -908,8 +1016,11 @@
       <c r="D36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43964</v>
       </c>
@@ -922,8 +1033,11 @@
       <c r="D37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43965</v>
       </c>
@@ -936,8 +1050,11 @@
       <c r="D38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43966</v>
       </c>
@@ -950,8 +1067,11 @@
       <c r="D39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43967</v>
       </c>
@@ -964,8 +1084,11 @@
       <c r="D40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43968</v>
       </c>
@@ -978,8 +1101,11 @@
       <c r="D41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43969</v>
       </c>
@@ -992,8 +1118,11 @@
       <c r="D42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43970</v>
       </c>
@@ -1006,8 +1135,11 @@
       <c r="D43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43971</v>
       </c>
@@ -1020,8 +1152,11 @@
       <c r="D44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43972</v>
       </c>
@@ -1034,8 +1169,11 @@
       <c r="D45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43973</v>
       </c>
@@ -1048,8 +1186,11 @@
       <c r="D46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43974</v>
       </c>
@@ -1062,8 +1203,11 @@
       <c r="D47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43975</v>
       </c>
@@ -1076,8 +1220,11 @@
       <c r="D48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43976</v>
       </c>
@@ -1090,8 +1237,11 @@
       <c r="D49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43977</v>
       </c>
@@ -1104,8 +1254,11 @@
       <c r="D50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43978</v>
       </c>
@@ -1118,8 +1271,11 @@
       <c r="D51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43979</v>
       </c>
@@ -1132,8 +1288,11 @@
       <c r="D52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43980</v>
       </c>
@@ -1146,8 +1305,11 @@
       <c r="D53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43981</v>
       </c>
@@ -1160,8 +1322,11 @@
       <c r="D54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43982</v>
       </c>
@@ -1174,8 +1339,11 @@
       <c r="D55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43983</v>
       </c>
@@ -1188,8 +1356,11 @@
       <c r="D56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43984</v>
       </c>
@@ -1202,8 +1373,11 @@
       <c r="D57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43985</v>
       </c>
@@ -1216,8 +1390,11 @@
       <c r="D58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43986</v>
       </c>
@@ -1230,8 +1407,11 @@
       <c r="D59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43987</v>
       </c>
@@ -1244,8 +1424,11 @@
       <c r="D60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43988</v>
       </c>
@@ -1258,8 +1441,11 @@
       <c r="D61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43989</v>
       </c>
@@ -1272,8 +1458,11 @@
       <c r="D62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43990</v>
       </c>
@@ -1286,8 +1475,11 @@
       <c r="D63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43991</v>
       </c>
@@ -1300,8 +1492,11 @@
       <c r="D64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>43992</v>
       </c>
@@ -1314,8 +1509,11 @@
       <c r="D65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>43993</v>
       </c>
@@ -1328,8 +1526,11 @@
       <c r="D66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>43994</v>
       </c>
@@ -1342,8 +1543,11 @@
       <c r="D67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>43995</v>
       </c>
@@ -1356,8 +1560,11 @@
       <c r="D68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>43996</v>
       </c>
@@ -1370,8 +1577,11 @@
       <c r="D69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>43997</v>
       </c>
@@ -1384,8 +1594,11 @@
       <c r="D70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>43998</v>
       </c>
@@ -1398,8 +1611,11 @@
       <c r="D71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>43999</v>
       </c>
@@ -1412,8 +1628,11 @@
       <c r="D72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>44000</v>
       </c>
@@ -1426,8 +1645,11 @@
       <c r="D73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>44001</v>
       </c>
@@ -1440,8 +1662,11 @@
       <c r="D74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>44002</v>
       </c>
@@ -1454,8 +1679,11 @@
       <c r="D75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>44003</v>
       </c>
@@ -1468,8 +1696,11 @@
       <c r="D76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>44004</v>
       </c>
@@ -1482,8 +1713,11 @@
       <c r="D77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>44005</v>
       </c>
@@ -1496,8 +1730,11 @@
       <c r="D78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>44006</v>
       </c>
@@ -1510,8 +1747,11 @@
       <c r="D79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>44007</v>
       </c>
@@ -1524,8 +1764,11 @@
       <c r="D80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>44008</v>
       </c>
@@ -1538,8 +1781,11 @@
       <c r="D81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>44009</v>
       </c>
@@ -1552,8 +1798,11 @@
       <c r="D82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>44010</v>
       </c>
@@ -1566,8 +1815,11 @@
       <c r="D83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>44011</v>
       </c>
@@ -1580,8 +1832,11 @@
       <c r="D84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>44012</v>
       </c>
@@ -1594,8 +1849,11 @@
       <c r="D85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>44013</v>
       </c>
@@ -1608,8 +1866,11 @@
       <c r="D86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>44014</v>
       </c>
@@ -1622,8 +1883,11 @@
       <c r="D87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>44015</v>
       </c>
@@ -1636,8 +1900,11 @@
       <c r="D88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>44016</v>
       </c>
@@ -1650,8 +1917,11 @@
       <c r="D89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>44017</v>
       </c>
@@ -1664,8 +1934,11 @@
       <c r="D90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>44018</v>
       </c>
@@ -1678,8 +1951,11 @@
       <c r="D91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>44019</v>
       </c>
@@ -1692,8 +1968,11 @@
       <c r="D92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>44020</v>
       </c>
@@ -1706,8 +1985,11 @@
       <c r="D93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>44021</v>
       </c>
@@ -1720,8 +2002,11 @@
       <c r="D94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>44022</v>
       </c>
@@ -1734,8 +2019,11 @@
       <c r="D95">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>44023</v>
       </c>
@@ -1748,8 +2036,11 @@
       <c r="D96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>44024</v>
       </c>
@@ -1762,8 +2053,11 @@
       <c r="D97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>44025</v>
       </c>
@@ -1776,8 +2070,11 @@
       <c r="D98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>44026</v>
       </c>
@@ -1790,8 +2087,11 @@
       <c r="D99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>44027</v>
       </c>
@@ -1804,8 +2104,11 @@
       <c r="D100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>44028</v>
       </c>
@@ -1818,8 +2121,11 @@
       <c r="D101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>44029</v>
       </c>
@@ -1832,8 +2138,11 @@
       <c r="D102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>44030</v>
       </c>
@@ -1846,8 +2155,11 @@
       <c r="D103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>44031</v>
       </c>
@@ -1860,8 +2172,11 @@
       <c r="D104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>44032</v>
       </c>
@@ -1874,8 +2189,11 @@
       <c r="D105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>44033</v>
       </c>
@@ -1888,8 +2206,11 @@
       <c r="D106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>44034</v>
       </c>
@@ -1902,8 +2223,11 @@
       <c r="D107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>44035</v>
       </c>
@@ -1916,8 +2240,11 @@
       <c r="D108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>44036</v>
       </c>
@@ -1930,8 +2257,11 @@
       <c r="D109">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>44037</v>
       </c>
@@ -1944,8 +2274,11 @@
       <c r="D110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>44038</v>
       </c>
@@ -1958,8 +2291,11 @@
       <c r="D111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>44039</v>
       </c>
@@ -1972,8 +2308,11 @@
       <c r="D112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>44040</v>
       </c>
@@ -1986,8 +2325,11 @@
       <c r="D113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>44041</v>
       </c>
@@ -2000,8 +2342,11 @@
       <c r="D114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>44042</v>
       </c>
@@ -2014,8 +2359,11 @@
       <c r="D115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>44043</v>
       </c>
@@ -2028,8 +2376,11 @@
       <c r="D116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>44044</v>
       </c>
@@ -2042,8 +2393,11 @@
       <c r="D117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>44045</v>
       </c>
@@ -2056,8 +2410,11 @@
       <c r="D118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>44046</v>
       </c>
@@ -2070,8 +2427,11 @@
       <c r="D119">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>44047</v>
       </c>
@@ -2084,8 +2444,11 @@
       <c r="D120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>44048</v>
       </c>
@@ -2098,8 +2461,11 @@
       <c r="D121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>44049</v>
       </c>
@@ -2112,8 +2478,11 @@
       <c r="D122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E122" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>44050</v>
       </c>
@@ -2126,8 +2495,11 @@
       <c r="D123">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>44051</v>
       </c>
@@ -2140,8 +2512,11 @@
       <c r="D124">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E124" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>44052</v>
       </c>
@@ -2154,8 +2529,11 @@
       <c r="D125">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>44053</v>
       </c>
@@ -2168,8 +2546,11 @@
       <c r="D126">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>44054</v>
       </c>
@@ -2182,8 +2563,11 @@
       <c r="D127">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>44055</v>
       </c>
@@ -2196,8 +2580,11 @@
       <c r="D128">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>44056</v>
       </c>
@@ -2210,8 +2597,11 @@
       <c r="D129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E129" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>44057</v>
       </c>
@@ -2224,8 +2614,11 @@
       <c r="D130">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>44058</v>
       </c>
@@ -2238,8 +2631,11 @@
       <c r="D131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>44059</v>
       </c>
@@ -2252,8 +2648,11 @@
       <c r="D132">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E132" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>44060</v>
       </c>
@@ -2266,8 +2665,11 @@
       <c r="D133">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>44061</v>
       </c>
@@ -2280,8 +2682,11 @@
       <c r="D134">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>44062</v>
       </c>
@@ -2294,8 +2699,11 @@
       <c r="D135">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>44063</v>
       </c>
@@ -2308,8 +2716,11 @@
       <c r="D136">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E136" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>44064</v>
       </c>
@@ -2322,8 +2733,11 @@
       <c r="D137">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E137" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>44065</v>
       </c>
@@ -2336,8 +2750,11 @@
       <c r="D138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>44066</v>
       </c>
@@ -2350,8 +2767,11 @@
       <c r="D139">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E139" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>44067</v>
       </c>
@@ -2364,8 +2784,11 @@
       <c r="D140">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E140" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>44068</v>
       </c>
@@ -2378,8 +2801,11 @@
       <c r="D141">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>44069</v>
       </c>
@@ -2392,8 +2818,11 @@
       <c r="D142">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>44070</v>
       </c>
@@ -2406,8 +2835,11 @@
       <c r="D143">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E143" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>44071</v>
       </c>
@@ -2420,8 +2852,11 @@
       <c r="D144">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>44072</v>
       </c>
@@ -2434,8 +2869,11 @@
       <c r="D145">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>44073</v>
       </c>
@@ -2448,8 +2886,11 @@
       <c r="D146">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>44074</v>
       </c>
@@ -2462,8 +2903,11 @@
       <c r="D147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E147" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>44075</v>
       </c>
@@ -2476,8 +2920,11 @@
       <c r="D148">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>44076</v>
       </c>
@@ -2490,8 +2937,11 @@
       <c r="D149">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>44077</v>
       </c>
@@ -2504,8 +2954,11 @@
       <c r="D150">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>44078</v>
       </c>
@@ -2518,8 +2971,11 @@
       <c r="D151">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E151" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>44079</v>
       </c>
@@ -2532,8 +2988,11 @@
       <c r="D152">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>44080</v>
       </c>
@@ -2546,8 +3005,11 @@
       <c r="D153">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E153" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>44081</v>
       </c>
@@ -2560,8 +3022,11 @@
       <c r="D154">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E154" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>44082</v>
       </c>
@@ -2574,8 +3039,11 @@
       <c r="D155">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E155" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>44083</v>
       </c>
@@ -2588,8 +3056,11 @@
       <c r="D156">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E156" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>44084</v>
       </c>
@@ -2602,8 +3073,11 @@
       <c r="D157">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>44085</v>
       </c>
@@ -2616,8 +3090,11 @@
       <c r="D158">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E158" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>44086</v>
       </c>
@@ -2630,8 +3107,11 @@
       <c r="D159">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E159" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>44087</v>
       </c>
@@ -2644,8 +3124,11 @@
       <c r="D160">
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>44088</v>
       </c>
@@ -2658,8 +3141,11 @@
       <c r="D161">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>44089</v>
       </c>
@@ -2672,8 +3158,11 @@
       <c r="D162">
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E162" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>44090</v>
       </c>
@@ -2686,8 +3175,11 @@
       <c r="D163">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E163" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>44091</v>
       </c>
@@ -2700,8 +3192,11 @@
       <c r="D164">
         <v>1</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E164" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>44092</v>
       </c>
@@ -2714,8 +3209,11 @@
       <c r="D165">
         <v>1</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E165" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>44093</v>
       </c>
@@ -2728,8 +3226,11 @@
       <c r="D166">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E166" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>44094</v>
       </c>
@@ -2742,8 +3243,11 @@
       <c r="D167">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E167" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>44095</v>
       </c>
@@ -2756,8 +3260,11 @@
       <c r="D168">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E168" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>44096</v>
       </c>
@@ -2770,8 +3277,11 @@
       <c r="D169">
         <v>1</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E169" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>44097</v>
       </c>
@@ -2784,8 +3294,11 @@
       <c r="D170">
         <v>1</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E170" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>44098</v>
       </c>
@@ -2798,8 +3311,11 @@
       <c r="D171">
         <v>1</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E171" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>44099</v>
       </c>
@@ -2812,8 +3328,11 @@
       <c r="D172">
         <v>1</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E172" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>44100</v>
       </c>
@@ -2826,8 +3345,11 @@
       <c r="D173">
         <v>1</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E173" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>44101</v>
       </c>
@@ -2840,8 +3362,11 @@
       <c r="D174">
         <v>1</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E174" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>44102</v>
       </c>
@@ -2854,8 +3379,11 @@
       <c r="D175">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E175" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>44103</v>
       </c>
@@ -2868,8 +3396,11 @@
       <c r="D176">
         <v>1</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E176" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>44104</v>
       </c>
@@ -2882,8 +3413,11 @@
       <c r="D177">
         <v>1</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E177" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>44105</v>
       </c>
@@ -2896,8 +3430,11 @@
       <c r="D178">
         <v>1</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E178" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>44106</v>
       </c>
@@ -2910,8 +3447,11 @@
       <c r="D179">
         <v>1</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E179" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>44107</v>
       </c>
@@ -2924,8 +3464,11 @@
       <c r="D180">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E180" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>44108</v>
       </c>
@@ -2938,8 +3481,11 @@
       <c r="D181">
         <v>1</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E181" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>44109</v>
       </c>
@@ -2952,8 +3498,11 @@
       <c r="D182">
         <v>1</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E182" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>44110</v>
       </c>
@@ -2966,8 +3515,11 @@
       <c r="D183">
         <v>1</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E183" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>44111</v>
       </c>
@@ -2980,8 +3532,11 @@
       <c r="D184">
         <v>1</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E184" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>44112</v>
       </c>
@@ -2994,8 +3549,11 @@
       <c r="D185">
         <v>1</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E185" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>44113</v>
       </c>
@@ -3008,8 +3566,11 @@
       <c r="D186">
         <v>1</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E186" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>44114</v>
       </c>
@@ -3022,8 +3583,11 @@
       <c r="D187">
         <v>1</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E187" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>44115</v>
       </c>
@@ -3036,8 +3600,11 @@
       <c r="D188">
         <v>1</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E188" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>44116</v>
       </c>
@@ -3050,8 +3617,11 @@
       <c r="D189">
         <v>1</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E189" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>44117</v>
       </c>
@@ -3064,8 +3634,11 @@
       <c r="D190">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E190" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>44118</v>
       </c>
@@ -3078,8 +3651,11 @@
       <c r="D191">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E191" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>44119</v>
       </c>
@@ -3092,8 +3668,11 @@
       <c r="D192">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E192" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>44120</v>
       </c>
@@ -3106,8 +3685,11 @@
       <c r="D193">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E193" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>44121</v>
       </c>
@@ -3120,8 +3702,11 @@
       <c r="D194">
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E194" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>44122</v>
       </c>
@@ -3134,8 +3719,11 @@
       <c r="D195">
         <v>1</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E195" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>44123</v>
       </c>
@@ -3148,8 +3736,11 @@
       <c r="D196">
         <v>1</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E196" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>44124</v>
       </c>
@@ -3162,8 +3753,11 @@
       <c r="D197">
         <v>1</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E197" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>44125</v>
       </c>
@@ -3176,8 +3770,11 @@
       <c r="D198">
         <v>1</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E198" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>44126</v>
       </c>
@@ -3190,8 +3787,11 @@
       <c r="D199">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E199" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>44127</v>
       </c>
@@ -3204,8 +3804,11 @@
       <c r="D200">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E200" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>44128</v>
       </c>
@@ -3218,8 +3821,11 @@
       <c r="D201">
         <v>1</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E201" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>44129</v>
       </c>
@@ -3232,8 +3838,11 @@
       <c r="D202">
         <v>1</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E202" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>44130</v>
       </c>
@@ -3246,8 +3855,11 @@
       <c r="D203">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E203" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>44131</v>
       </c>
@@ -3260,8 +3872,11 @@
       <c r="D204">
         <v>1</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E204" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>44132</v>
       </c>
@@ -3274,8 +3889,11 @@
       <c r="D205">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E205" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>44133</v>
       </c>
@@ -3288,8 +3906,11 @@
       <c r="D206">
         <v>1</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E206" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>44134</v>
       </c>
@@ -3302,8 +3923,11 @@
       <c r="D207">
         <v>1</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E207" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>44135</v>
       </c>
@@ -3316,8 +3940,11 @@
       <c r="D208">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E208" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>44136</v>
       </c>
@@ -3330,8 +3957,11 @@
       <c r="D209">
         <v>1</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E209" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>44137</v>
       </c>
@@ -3344,8 +3974,11 @@
       <c r="D210">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E210" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>44138.416666666664</v>
       </c>
@@ -3358,8 +3991,11 @@
       <c r="D211">
         <v>2</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E211" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>44138.5</v>
       </c>
@@ -3372,8 +4008,11 @@
       <c r="D212">
         <v>2</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E212" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>44138.552083333336</v>
       </c>
@@ -3386,8 +4025,11 @@
       <c r="D213">
         <v>2</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E213" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>44138.583333333336</v>
       </c>
@@ -3400,8 +4042,11 @@
       <c r="D214">
         <v>2</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E214" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>44138.604166666664</v>
       </c>
@@ -3414,8 +4059,11 @@
       <c r="D215">
         <v>2</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E215" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>44138.65625</v>
       </c>
@@ -3428,8 +4076,11 @@
       <c r="D216">
         <v>2</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E216" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>44138.75</v>
       </c>
@@ -3442,8 +4093,11 @@
       <c r="D217">
         <v>2</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E217" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>44138.791666666664</v>
       </c>
@@ -3456,8 +4110,11 @@
       <c r="D218">
         <v>2</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E218" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>44138.798611111109</v>
       </c>
@@ -3470,8 +4127,11 @@
       <c r="D219">
         <v>2</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E219" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>44138.805555555555</v>
       </c>
@@ -3484,8 +4144,11 @@
       <c r="D220">
         <v>2</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E220" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>44138.809027777781</v>
       </c>
@@ -3498,8 +4161,11 @@
       <c r="D221">
         <v>2</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E221" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>44138.8125</v>
       </c>
@@ -3512,8 +4178,11 @@
       <c r="D222">
         <v>2</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E222" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>44138.815972222219</v>
       </c>
@@ -3526,8 +4195,11 @@
       <c r="D223">
         <v>2</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E223" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>44138.822916666664</v>
       </c>
@@ -3540,8 +4212,11 @@
       <c r="D224">
         <v>2</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E224" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>44138.826388888891</v>
       </c>
@@ -3554,8 +4229,11 @@
       <c r="D225">
         <v>2</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E225" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>44138.833333333336</v>
       </c>
@@ -3568,8 +4246,11 @@
       <c r="D226">
         <v>2</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E226" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>44138.84375</v>
       </c>
@@ -3582,8 +4263,11 @@
       <c r="D227">
         <v>2</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E227" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>44138.850694444445</v>
       </c>
@@ -3596,8 +4280,11 @@
       <c r="D228">
         <v>2</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E228" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>44138.857638888891</v>
       </c>
@@ -3610,8 +4297,11 @@
       <c r="D229">
         <v>2</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E229" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>44138.864583333336</v>
       </c>
@@ -3624,8 +4314,11 @@
       <c r="D230">
         <v>2</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E230" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>44138.868055555555</v>
       </c>
@@ -3638,8 +4331,11 @@
       <c r="D231">
         <v>2</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E231" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>44138.875</v>
       </c>
@@ -3652,8 +4348,11 @@
       <c r="D232">
         <v>2</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E232" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>44138.888888888891</v>
       </c>
@@ -3666,8 +4365,11 @@
       <c r="D233">
         <v>2</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E233" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>44138.892361111109</v>
       </c>
@@ -3680,8 +4382,11 @@
       <c r="D234">
         <v>2</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E234" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>44138.895833333336</v>
       </c>
@@ -3694,8 +4399,11 @@
       <c r="D235">
         <v>2</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E235" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>44138.899305555555</v>
       </c>
@@ -3708,8 +4416,11 @@
       <c r="D236">
         <v>2</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E236" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>44138.902777777781</v>
       </c>
@@ -3722,8 +4433,11 @@
       <c r="D237">
         <v>2</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E237" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>44138.916666666664</v>
       </c>
@@ -3736,8 +4450,11 @@
       <c r="D238">
         <v>2</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E238" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>44138.923611111109</v>
       </c>
@@ -3750,8 +4467,11 @@
       <c r="D239">
         <v>2</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E239" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>44138.930555555555</v>
       </c>
@@ -3764,8 +4484,11 @@
       <c r="D240">
         <v>2</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E240" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>44138.940972222219</v>
       </c>
@@ -3778,8 +4501,11 @@
       <c r="D241">
         <v>2</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E241" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>44138.947916666664</v>
       </c>
@@ -3792,8 +4518,11 @@
       <c r="D242">
         <v>2</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E242" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>44138.958333333336</v>
       </c>
@@ -3806,8 +4535,11 @@
       <c r="D243">
         <v>2</v>
       </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E243" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>44138.961805555555</v>
       </c>
@@ -3820,8 +4552,11 @@
       <c r="D244">
         <v>2</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E244" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>44138.96875</v>
       </c>
@@ -3834,8 +4569,11 @@
       <c r="D245">
         <v>2</v>
       </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E245" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>44138.979166666664</v>
       </c>
@@ -3848,8 +4586,11 @@
       <c r="D246">
         <v>2</v>
       </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E246" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>44138.986111111109</v>
       </c>
@@ -3862,8 +4603,11 @@
       <c r="D247">
         <v>2</v>
       </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E247" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>44138.993055555555</v>
       </c>
@@ -3876,8 +4620,11 @@
       <c r="D248">
         <v>2</v>
       </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E248" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>44139</v>
       </c>
@@ -3890,8 +4637,11 @@
       <c r="D249">
         <v>2</v>
       </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E249" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>44139.006944444445</v>
       </c>
@@ -3904,8 +4654,11 @@
       <c r="D250">
         <v>2</v>
       </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E250" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>44139.010416666664</v>
       </c>
@@ -3918,8 +4671,11 @@
       <c r="D251">
         <v>2</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E251" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>44139.020833333336</v>
       </c>
@@ -3932,8 +4688,11 @@
       <c r="D252">
         <v>2</v>
       </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E252" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>44139.034722222219</v>
       </c>
@@ -3946,8 +4705,11 @@
       <c r="D253">
         <v>2</v>
       </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E253" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>44139.041666666664</v>
       </c>
@@ -3960,8 +4722,11 @@
       <c r="D254">
         <v>2</v>
       </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E254" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>44139.048611111109</v>
       </c>
@@ -3974,8 +4739,11 @@
       <c r="D255">
         <v>2</v>
       </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E255" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>44139.375</v>
       </c>
@@ -3988,8 +4756,11 @@
       <c r="D256">
         <v>2</v>
       </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E256" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>44139.416666666664</v>
       </c>
@@ -4002,8 +4773,11 @@
       <c r="D257">
         <v>2</v>
       </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E257" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>44139.458333333336</v>
       </c>
@@ -4016,8 +4790,11 @@
       <c r="D258">
         <v>2</v>
       </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E258" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>44139.510416666664</v>
       </c>
@@ -4030,8 +4807,11 @@
       <c r="D259">
         <v>2</v>
       </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E259" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>44139.5625</v>
       </c>
@@ -4044,8 +4824,11 @@
       <c r="D260">
         <v>2</v>
       </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E260" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>44139.565972222219</v>
       </c>
@@ -4058,8 +4841,11 @@
       <c r="D261">
         <v>1</v>
       </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E261" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>44139.638888888891</v>
       </c>
@@ -4072,8 +4858,11 @@
       <c r="D262">
         <v>1</v>
       </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E262" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>44139.708333333336</v>
       </c>
@@ -4086,8 +4875,11 @@
       <c r="D263">
         <v>1</v>
       </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E263" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>44140.017361111109</v>
       </c>
@@ -4100,8 +4892,11 @@
       <c r="D264">
         <v>1</v>
       </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E264" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>44140.430555555555</v>
       </c>
@@ -4114,8 +4909,11 @@
       <c r="D265">
         <v>1</v>
       </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E265" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>44140.652777777781</v>
       </c>
@@ -4128,8 +4926,11 @@
       <c r="D266">
         <v>1</v>
       </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E266" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>44141.388888888891</v>
       </c>
@@ -4141,6 +4942,9 @@
       </c>
       <c r="D267">
         <v>1</v>
+      </c>
+      <c r="E267" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
visualization complete, now need to deploy on heroku
</commit_message>
<xml_diff>
--- a/src/data/Election Odds Raw.xlsx
+++ b/src/data/Election Odds Raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Developer/2020-Election-Odds-Tracker/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9BA914-1C24-FF43-884A-E6C2A322D1C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017BD8B0-736C-7249-ACCB-3A1861579CDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29400" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{E91F47DA-0CB0-014E-85A8-F4E87909AA65}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{E91F47DA-0CB0-014E-85A8-F4E87909AA65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>date</t>
   </si>
@@ -48,6 +48,114 @@
   </si>
   <si>
     <t>pre_first_results</t>
+  </si>
+  <si>
+    <t>U.S. COVID-19 deaths surpass 100,000</t>
+  </si>
+  <si>
+    <t>notes_source</t>
+  </si>
+  <si>
+    <t>Peak of Black Lives Matter Protests: 500,000 people in 550 cities</t>
+  </si>
+  <si>
+    <t>Republican National Convention begins through Aug. 27</t>
+  </si>
+  <si>
+    <t>Democratic National Convention begins through Aug. 20. Biden certified as Democratic Nominee</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Vice Presidential Debate</t>
+  </si>
+  <si>
+    <t>Second and final Presidential Debate</t>
+  </si>
+  <si>
+    <t>First Presidential Debate</t>
+  </si>
+  <si>
+    <t>3,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polls close in VT, KY, IN, VA, GA, SC. First results in NH, FL. AP calls KY for Trump, VT for Biden. </t>
+  </si>
+  <si>
+    <t>Polls close in WV, OH, NC. AP calls WV for Trump</t>
+  </si>
+  <si>
+    <t>First results in IN, KY</t>
+  </si>
+  <si>
+    <t>Polls close in AK, HI</t>
+  </si>
+  <si>
+    <t>AP calls VA for Biden</t>
+  </si>
+  <si>
+    <t>AP calls SC for Trump</t>
+  </si>
+  <si>
+    <t>Polls close in NH, ME, MA, CT, RI, NJ, PA, MD, DE, DC, IL, MO, OK, TN, MS, AL, FL. First Results in TX, ND, SD, KS, MI. AP calls AL, MI, TN, OK for Trump, CT, DE, IL, MD, MA, NJ, RI for Biden</t>
+  </si>
+  <si>
+    <t>Polls close in AR. AP calls AR for Trump</t>
+  </si>
+  <si>
+    <t>AP calls IN for Trump</t>
+  </si>
+  <si>
+    <t>Polls close in NY, MI, WI, MN, ND, SD, WY, NE, CO, AZ, NM, TX, LA, KS. AP calls ND, SD, WY, LA, NE for Trump, NY, NM for Biden.</t>
+  </si>
+  <si>
+    <t>AP calls DC for Biden</t>
+  </si>
+  <si>
+    <t>AP calls CO for Biden</t>
+  </si>
+  <si>
+    <t>Polls close in NV, UT, MT, IA. First results in ID. AP calls KS for Trump.</t>
+  </si>
+  <si>
+    <t>AP calls MO for Trump</t>
+  </si>
+  <si>
+    <t>Polls close in WA, OR, ID, CA. AP calls ID for trump, CA, OR, WA for Biden</t>
+  </si>
+  <si>
+    <t>AP calls UT for Trump</t>
+  </si>
+  <si>
+    <t>AP calls HI for Biden</t>
+  </si>
+  <si>
+    <t>AP calls MN for Biden</t>
+  </si>
+  <si>
+    <t>AP calls MT, IA, OH, FL for Trump</t>
+  </si>
+  <si>
+    <t>AP calls AZ, ME for Biden</t>
+  </si>
+  <si>
+    <t>AP calls WI for Biden</t>
+  </si>
+  <si>
+    <t>AP calls MI for Biden</t>
+  </si>
+  <si>
+    <t>Biden overtakes Trump in WI, MI</t>
+  </si>
+  <si>
+    <t>Bernie Sanders suspends campaign, all but assuring Joe Biden will be the Democratic nominee</t>
+  </si>
+  <si>
+    <t>U.S. COVID-19 deaths surpass 200,000</t>
+  </si>
+  <si>
+    <t>Trump tests positive for COVID-19</t>
   </si>
 </sst>
 </file>
@@ -400,15 +508,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E09FD95-8348-4048-A5D2-30A6965E257B}">
-  <dimension ref="A1:E267"/>
+  <dimension ref="A1:G267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E218" sqref="E218:E267"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="G256" sqref="G256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="98.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,8 +535,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43929</v>
       </c>
@@ -441,8 +558,14 @@
       <c r="E2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43930</v>
       </c>
@@ -459,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43931</v>
       </c>
@@ -476,7 +599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43932</v>
       </c>
@@ -493,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43933</v>
       </c>
@@ -510,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43934</v>
       </c>
@@ -527,7 +650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43935</v>
       </c>
@@ -544,7 +667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43936</v>
       </c>
@@ -561,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43937</v>
       </c>
@@ -578,7 +701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43938</v>
       </c>
@@ -595,7 +718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43939</v>
       </c>
@@ -612,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43940</v>
       </c>
@@ -629,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43941</v>
       </c>
@@ -646,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43942</v>
       </c>
@@ -663,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43943</v>
       </c>
@@ -1224,7 +1347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43976</v>
       </c>
@@ -1241,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43977</v>
       </c>
@@ -1258,7 +1381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43978</v>
       </c>
@@ -1274,8 +1397,14 @@
       <c r="E51" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43979</v>
       </c>
@@ -1292,7 +1421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43980</v>
       </c>
@@ -1309,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43981</v>
       </c>
@@ -1326,7 +1455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43982</v>
       </c>
@@ -1343,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43983</v>
       </c>
@@ -1360,7 +1489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43984</v>
       </c>
@@ -1377,7 +1506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43985</v>
       </c>
@@ -1394,7 +1523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43986</v>
       </c>
@@ -1411,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43987</v>
       </c>
@@ -1428,7 +1557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43988</v>
       </c>
@@ -1444,8 +1573,14 @@
       <c r="E61" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43989</v>
       </c>
@@ -1462,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43990</v>
       </c>
@@ -1479,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43991</v>
       </c>
@@ -2584,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>44056</v>
       </c>
@@ -2601,7 +2736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>44057</v>
       </c>
@@ -2618,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>44058</v>
       </c>
@@ -2635,7 +2770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>44059</v>
       </c>
@@ -2652,7 +2787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>44060</v>
       </c>
@@ -2668,8 +2803,14 @@
       <c r="E133" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F133" t="s">
+        <v>9</v>
+      </c>
+      <c r="G133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>44061</v>
       </c>
@@ -2686,7 +2827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>44062</v>
       </c>
@@ -2703,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>44063</v>
       </c>
@@ -2720,7 +2861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>44064</v>
       </c>
@@ -2737,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>44065</v>
       </c>
@@ -2754,7 +2895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>44066</v>
       </c>
@@ -2771,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>44067</v>
       </c>
@@ -2787,8 +2928,14 @@
       <c r="E140" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F140" t="s">
+        <v>8</v>
+      </c>
+      <c r="G140">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>44068</v>
       </c>
@@ -2805,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>44069</v>
       </c>
@@ -2822,7 +2969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>44070</v>
       </c>
@@ -2839,7 +2986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>44071</v>
       </c>
@@ -3128,7 +3275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>44088</v>
       </c>
@@ -3145,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>44089</v>
       </c>
@@ -3162,7 +3309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>44090</v>
       </c>
@@ -3179,7 +3326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>44091</v>
       </c>
@@ -3196,7 +3343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>44092</v>
       </c>
@@ -3213,7 +3360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>44093</v>
       </c>
@@ -3230,7 +3377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>44094</v>
       </c>
@@ -3247,7 +3394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>44095</v>
       </c>
@@ -3264,7 +3411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>44096</v>
       </c>
@@ -3280,8 +3427,14 @@
       <c r="E169" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F169" t="s">
+        <v>39</v>
+      </c>
+      <c r="G169">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>44097</v>
       </c>
@@ -3298,7 +3451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>44098</v>
       </c>
@@ -3315,7 +3468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>44099</v>
       </c>
@@ -3332,7 +3485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>44100</v>
       </c>
@@ -3349,7 +3502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>44101</v>
       </c>
@@ -3366,7 +3519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>44102</v>
       </c>
@@ -3382,8 +3535,11 @@
       <c r="E175" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G175">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>44103</v>
       </c>
@@ -3399,8 +3555,11 @@
       <c r="E176" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F176" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>44104</v>
       </c>
@@ -3417,7 +3576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>44105</v>
       </c>
@@ -3433,8 +3592,11 @@
       <c r="E178" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G178">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>44106</v>
       </c>
@@ -3450,8 +3612,11 @@
       <c r="E179" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F179" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>44107</v>
       </c>
@@ -3468,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>44108</v>
       </c>
@@ -3485,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>44109</v>
       </c>
@@ -3502,7 +3667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>44110</v>
       </c>
@@ -3519,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>44111</v>
       </c>
@@ -3535,8 +3700,14 @@
       <c r="E184" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F184" t="s">
+        <v>11</v>
+      </c>
+      <c r="G184">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>44112</v>
       </c>
@@ -3553,7 +3724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>44113</v>
       </c>
@@ -3570,7 +3741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>44114</v>
       </c>
@@ -3587,7 +3758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>44115</v>
       </c>
@@ -3604,7 +3775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>44116</v>
       </c>
@@ -3621,7 +3792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>44117</v>
       </c>
@@ -3638,7 +3809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>44118</v>
       </c>
@@ -3655,7 +3826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>44119</v>
       </c>
@@ -3672,7 +3843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>44120</v>
       </c>
@@ -3689,7 +3860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>44121</v>
       </c>
@@ -3706,7 +3877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>44122</v>
       </c>
@@ -3723,7 +3894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>44123</v>
       </c>
@@ -3740,7 +3911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>44124</v>
       </c>
@@ -3757,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>44125</v>
       </c>
@@ -3774,7 +3945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>44126</v>
       </c>
@@ -3790,8 +3961,14 @@
       <c r="E199" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F199" t="s">
+        <v>12</v>
+      </c>
+      <c r="G199">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>44127</v>
       </c>
@@ -3808,7 +3985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>44128</v>
       </c>
@@ -3825,7 +4002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>44129</v>
       </c>
@@ -3842,7 +4019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>44130</v>
       </c>
@@ -3859,7 +4036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>44131</v>
       </c>
@@ -3876,7 +4053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>44132</v>
       </c>
@@ -3893,7 +4070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>44133</v>
       </c>
@@ -3910,7 +4087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>44134</v>
       </c>
@@ -3927,7 +4104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>44135</v>
       </c>
@@ -3944,7 +4121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>44136</v>
       </c>
@@ -3961,7 +4138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>44137</v>
       </c>
@@ -3978,7 +4155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>44138.416666666664</v>
       </c>
@@ -3995,7 +4172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>44138.5</v>
       </c>
@@ -4012,7 +4189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>44138.552083333336</v>
       </c>
@@ -4029,7 +4206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>44138.583333333336</v>
       </c>
@@ -4046,7 +4223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>44138.604166666664</v>
       </c>
@@ -4063,7 +4240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>44138.65625</v>
       </c>
@@ -4080,7 +4257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>44138.75</v>
       </c>
@@ -4094,10 +4271,16 @@
         <v>2</v>
       </c>
       <c r="E217" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F217" t="s">
+        <v>17</v>
+      </c>
+      <c r="G217">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>44138.791666666664</v>
       </c>
@@ -4113,8 +4296,14 @@
       <c r="E218" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F218" t="s">
+        <v>15</v>
+      </c>
+      <c r="G218" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>44138.798611111109</v>
       </c>
@@ -4131,7 +4320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>44138.805555555555</v>
       </c>
@@ -4148,7 +4337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>44138.809027777781</v>
       </c>
@@ -4165,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>44138.8125</v>
       </c>
@@ -4181,8 +4370,14 @@
       <c r="E222" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F222" t="s">
+        <v>16</v>
+      </c>
+      <c r="G222" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>44138.815972222219</v>
       </c>
@@ -4198,8 +4393,14 @@
       <c r="E223" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F223" t="s">
+        <v>19</v>
+      </c>
+      <c r="G223">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>44138.822916666664</v>
       </c>
@@ -4216,7 +4417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>44138.826388888891</v>
       </c>
@@ -4232,8 +4433,14 @@
       <c r="E225" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F225" t="s">
+        <v>20</v>
+      </c>
+      <c r="G225">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>44138.833333333336</v>
       </c>
@@ -4249,8 +4456,14 @@
       <c r="E226" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F226" t="s">
+        <v>21</v>
+      </c>
+      <c r="G226" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>44138.84375</v>
       </c>
@@ -4267,7 +4480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>44138.850694444445</v>
       </c>
@@ -4284,7 +4497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>44138.857638888891</v>
       </c>
@@ -4300,8 +4513,14 @@
       <c r="E229" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F229" t="s">
+        <v>22</v>
+      </c>
+      <c r="G229" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>44138.864583333336</v>
       </c>
@@ -4318,7 +4537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>44138.868055555555</v>
       </c>
@@ -4334,8 +4553,14 @@
       <c r="E231" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F231" t="s">
+        <v>23</v>
+      </c>
+      <c r="G231">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>44138.875</v>
       </c>
@@ -4351,8 +4576,14 @@
       <c r="E232" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F232" t="s">
+        <v>24</v>
+      </c>
+      <c r="G232" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>44138.888888888891</v>
       </c>
@@ -4369,7 +4600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>44138.892361111109</v>
       </c>
@@ -4385,8 +4616,14 @@
       <c r="E234" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F234" t="s">
+        <v>25</v>
+      </c>
+      <c r="G234">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>44138.895833333336</v>
       </c>
@@ -4403,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>44138.899305555555</v>
       </c>
@@ -4419,8 +4656,14 @@
       <c r="E236" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F236" t="s">
+        <v>26</v>
+      </c>
+      <c r="G236">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>44138.902777777781</v>
       </c>
@@ -4437,7 +4680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>44138.916666666664</v>
       </c>
@@ -4453,8 +4696,14 @@
       <c r="E238" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F238" t="s">
+        <v>27</v>
+      </c>
+      <c r="G238" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>44138.923611111109</v>
       </c>
@@ -4471,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>44138.930555555555</v>
       </c>
@@ -4488,7 +4737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>44138.940972222219</v>
       </c>
@@ -4504,8 +4753,14 @@
       <c r="E241" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F241" t="s">
+        <v>28</v>
+      </c>
+      <c r="G241">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>44138.947916666664</v>
       </c>
@@ -4522,7 +4777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>44138.958333333336</v>
       </c>
@@ -4538,8 +4793,14 @@
       <c r="E243" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F243" t="s">
+        <v>29</v>
+      </c>
+      <c r="G243" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>44138.961805555555</v>
       </c>
@@ -4555,8 +4816,14 @@
       <c r="E244" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F244" t="s">
+        <v>30</v>
+      </c>
+      <c r="G244">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>44138.96875</v>
       </c>
@@ -4573,7 +4840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>44138.979166666664</v>
       </c>
@@ -4590,7 +4857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>44138.986111111109</v>
       </c>
@@ -4607,7 +4874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>44138.993055555555</v>
       </c>
@@ -4624,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>44139</v>
       </c>
@@ -4640,8 +4907,14 @@
       <c r="E249" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F249" t="s">
+        <v>18</v>
+      </c>
+      <c r="G249">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>44139.006944444445</v>
       </c>
@@ -4657,8 +4930,14 @@
       <c r="E250" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F250" t="s">
+        <v>31</v>
+      </c>
+      <c r="G250">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>44139.010416666664</v>
       </c>
@@ -4674,8 +4953,14 @@
       <c r="E251" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F251" t="s">
+        <v>32</v>
+      </c>
+      <c r="G251">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>44139.020833333336</v>
       </c>
@@ -4691,8 +4976,14 @@
       <c r="E252" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F252" t="s">
+        <v>33</v>
+      </c>
+      <c r="G252">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>44139.034722222219</v>
       </c>
@@ -4709,7 +5000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>44139.041666666664</v>
       </c>
@@ -4726,7 +5017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>44139.048611111109</v>
       </c>
@@ -4742,8 +5033,14 @@
       <c r="E255" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F255" t="s">
+        <v>34</v>
+      </c>
+      <c r="G255">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>44139.375</v>
       </c>
@@ -4759,8 +5056,14 @@
       <c r="E256" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F256" t="s">
+        <v>37</v>
+      </c>
+      <c r="G256">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>44139.416666666664</v>
       </c>
@@ -4777,7 +5080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>44139.458333333336</v>
       </c>
@@ -4794,7 +5097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>44139.510416666664</v>
       </c>
@@ -4811,7 +5114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>44139.5625</v>
       </c>
@@ -4828,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>44139.565972222219</v>
       </c>
@@ -4845,7 +5148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>44139.638888888891</v>
       </c>
@@ -4861,8 +5164,14 @@
       <c r="E262" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F262" t="s">
+        <v>35</v>
+      </c>
+      <c r="G262">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>44139.708333333336</v>
       </c>
@@ -4878,8 +5187,14 @@
       <c r="E263" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F263" t="s">
+        <v>36</v>
+      </c>
+      <c r="G263">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>44140.017361111109</v>
       </c>
@@ -4896,7 +5211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>44140.430555555555</v>
       </c>
@@ -4913,7 +5228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>44140.652777777781</v>
       </c>
@@ -4930,7 +5245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>44141.388888888891</v>
       </c>

</xml_diff>